<commit_message>
Handles float input without breaking stuff
</commit_message>
<xml_diff>
--- a/ans/result/1401CB01.xlsx
+++ b/ans/result/1401CB01.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="quiz" sheetId="1" state="visible" r:id="rId1"/>
@@ -83,67 +83,67 @@
     </border>
   </borders>
   <cellStyleXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="2" numFmtId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="3" numFmtId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1">
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="3" numFmtId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1">
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="4" numFmtId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1">
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="5" numFmtId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyAlignment="1">
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="6" numFmtId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyAlignment="1">
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="3">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="6">
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="5">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="7">
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="6">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="5">
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="7">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="4">
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="4">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
-    <cellStyle name="rtitleStyle" xfId="1" hidden="0"/>
-    <cellStyle name="ltitleStyle" xfId="2" hidden="0"/>
-    <cellStyle name="mtitleStyle" xfId="3" hidden="0"/>
-    <cellStyle name="absoluteStyle" xfId="4" hidden="0"/>
-    <cellStyle name="normalStyle" xfId="5" hidden="0"/>
-    <cellStyle name="correctStyle" xfId="6" hidden="0"/>
-    <cellStyle name="incorrectStyle" xfId="7" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle hidden="0" name="rtitleStyle" xfId="1"/>
+    <cellStyle hidden="0" name="ltitleStyle" xfId="2"/>
+    <cellStyle hidden="0" name="mtitleStyle" xfId="3"/>
+    <cellStyle hidden="0" name="absoluteStyle" xfId="4"/>
+    <cellStyle hidden="0" name="correctStyle" xfId="5"/>
+    <cellStyle hidden="0" name="incorrectStyle" xfId="6"/>
+    <cellStyle hidden="0" name="normalStyle" xfId="7"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -227,7 +227,7 @@
     <ext cx="6029325" cy="790575"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPr descr="Picture" id="1" name="Image 1"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
@@ -534,7 +534,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A5:H40"/>
+  <dimension ref="A5:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -542,11 +542,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="18" customWidth="1" min="1" max="1"/>
-    <col width="18" customWidth="1" min="2" max="2"/>
-    <col width="18" customWidth="1" min="3" max="3"/>
-    <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="18" customWidth="1" min="5" max="5"/>
+    <col customWidth="1" max="1" min="1" width="18"/>
+    <col customWidth="1" max="2" min="2" width="18"/>
+    <col customWidth="1" max="3" min="3" width="18"/>
+    <col customWidth="1" max="4" min="4" width="18"/>
+    <col customWidth="1" max="5" min="5" width="18"/>
   </cols>
   <sheetData>
     <row r="5">
@@ -617,37 +617,35 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="4" t="inlineStr">
         <is>
           <t>No.</t>
         </is>
       </c>
       <c r="B10" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="C10" s="6" t="n">
+        <v>14</v>
+      </c>
+      <c r="D10" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="C10" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" s="7" t="n">
-        <v>56</v>
-      </c>
       <c r="E10" s="7" t="n">
-        <v>56</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="4" t="inlineStr">
         <is>
           <t>Marking</t>
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="C11" s="6" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
+        <v>4</v>
+      </c>
+      <c r="C11" s="6" t="n">
+        <v>-1</v>
       </c>
       <c r="D11" s="7" t="n">
         <v>0</v>
@@ -655,21 +653,21 @@
       <c r="E11" s="4" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="4" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
       <c r="B12" s="5" t="n">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="C12" s="6" t="n">
-        <v>0</v>
+        <v>-14</v>
       </c>
       <c r="D12" s="7" t="n"/>
       <c r="E12" s="8" t="inlineStr">
         <is>
-          <t>Absent</t>
+          <t>42/112</t>
         </is>
       </c>
     </row>
@@ -694,400 +692,334 @@
           <t>Correct Ans</t>
         </is>
       </c>
-      <c r="G15" s="4" t="inlineStr">
-        <is>
-          <t>Student Ans</t>
-        </is>
-      </c>
-      <c r="H15" s="4" t="inlineStr">
-        <is>
-          <t>Correct Ans</t>
-        </is>
-      </c>
     </row>
     <row r="16">
-      <c r="A16" s="7" t="inlineStr"/>
+      <c r="A16" s="5" t="inlineStr">
+        <is>
+          <t>Option A</t>
+        </is>
+      </c>
       <c r="B16" s="8" t="inlineStr">
         <is>
           <t>Option A</t>
         </is>
       </c>
-      <c r="D16" s="7" t="inlineStr"/>
+      <c r="D16" s="5" t="inlineStr">
+        <is>
+          <t>Option A</t>
+        </is>
+      </c>
       <c r="E16" s="8" t="inlineStr">
         <is>
           <t>Option A</t>
         </is>
       </c>
-      <c r="G16" s="7" t="inlineStr"/>
-      <c r="H16" s="8" t="inlineStr">
+    </row>
+    <row r="17">
+      <c r="A17" s="6" t="inlineStr">
+        <is>
+          <t>Option C</t>
+        </is>
+      </c>
+      <c r="B17" s="8" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+      <c r="D17" s="5" t="inlineStr">
+        <is>
+          <t>Option C</t>
+        </is>
+      </c>
+      <c r="E17" s="8" t="inlineStr">
+        <is>
+          <t>Option C</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="5" t="inlineStr">
+        <is>
+          <t>Option B</t>
+        </is>
+      </c>
+      <c r="B18" s="8" t="inlineStr">
+        <is>
+          <t>Option B</t>
+        </is>
+      </c>
+      <c r="D18" s="5" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+      <c r="E18" s="8" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="5" t="inlineStr">
+        <is>
+          <t>Option C</t>
+        </is>
+      </c>
+      <c r="B19" s="8" t="inlineStr">
+        <is>
+          <t>Option C</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="6" t="inlineStr">
+        <is>
+          <t>Option C</t>
+        </is>
+      </c>
+      <c r="B20" s="8" t="inlineStr">
+        <is>
+          <t>Option B</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="5" t="inlineStr">
+        <is>
+          <t>Option C</t>
+        </is>
+      </c>
+      <c r="B21" s="8" t="inlineStr">
+        <is>
+          <t>Option C</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="5" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+      <c r="B22" s="8" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="6" t="inlineStr">
+        <is>
+          <t>Option C</t>
+        </is>
+      </c>
+      <c r="B23" s="8" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="6" t="inlineStr">
+        <is>
+          <t>Option C</t>
+        </is>
+      </c>
+      <c r="B24" s="8" t="inlineStr">
         <is>
           <t>Option A</t>
         </is>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="7" t="inlineStr"/>
-      <c r="B17" s="8" t="inlineStr">
-        <is>
-          <t>Option D</t>
-        </is>
-      </c>
-      <c r="D17" s="7" t="inlineStr"/>
-      <c r="E17" s="8" t="inlineStr">
-        <is>
-          <t>Option C</t>
-        </is>
-      </c>
-      <c r="G17" s="7" t="inlineStr"/>
-      <c r="H17" s="8" t="inlineStr">
-        <is>
-          <t>Option D</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="7" t="inlineStr"/>
-      <c r="B18" s="8" t="inlineStr">
+    <row r="25">
+      <c r="A25" s="6" t="inlineStr">
+        <is>
+          <t>Option C</t>
+        </is>
+      </c>
+      <c r="B25" s="8" t="inlineStr">
+        <is>
+          <t>Option A</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="5" t="inlineStr">
+        <is>
+          <t>Option C</t>
+        </is>
+      </c>
+      <c r="B26" s="8" t="inlineStr">
+        <is>
+          <t>Option C</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="5" t="inlineStr">
+        <is>
+          <t>Option A</t>
+        </is>
+      </c>
+      <c r="B27" s="8" t="inlineStr">
+        <is>
+          <t>Option A</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="6" t="inlineStr">
+        <is>
+          <t>Option C</t>
+        </is>
+      </c>
+      <c r="B28" s="8" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="6" t="inlineStr">
+        <is>
+          <t>Option C</t>
+        </is>
+      </c>
+      <c r="B29" s="8" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="6" t="inlineStr">
+        <is>
+          <t>Option C</t>
+        </is>
+      </c>
+      <c r="B30" s="8" t="inlineStr">
         <is>
           <t>Option B</t>
         </is>
       </c>
-      <c r="D18" s="7" t="inlineStr"/>
-      <c r="E18" s="8" t="inlineStr">
-        <is>
-          <t>Option D</t>
-        </is>
-      </c>
-      <c r="G18" s="7" t="inlineStr"/>
-      <c r="H18" s="8" t="inlineStr">
-        <is>
-          <t>Option D</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="7" t="inlineStr"/>
-      <c r="B19" s="8" t="inlineStr">
-        <is>
-          <t>Option C</t>
-        </is>
-      </c>
-      <c r="D19" s="7" t="inlineStr"/>
-      <c r="E19" s="8" t="inlineStr">
+    </row>
+    <row r="31">
+      <c r="A31" s="5" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+      <c r="B31" s="8" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="5" t="inlineStr">
+        <is>
+          <t>Option C</t>
+        </is>
+      </c>
+      <c r="B32" s="8" t="inlineStr">
+        <is>
+          <t>Option C</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="6" t="inlineStr">
+        <is>
+          <t>Option B</t>
+        </is>
+      </c>
+      <c r="B33" s="8" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="6" t="inlineStr">
+        <is>
+          <t>Option C</t>
+        </is>
+      </c>
+      <c r="B34" s="8" t="inlineStr">
+        <is>
+          <t>Option B</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="5" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+      <c r="B35" s="8" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="6" t="inlineStr">
+        <is>
+          <t>Option C</t>
+        </is>
+      </c>
+      <c r="B36" s="8" t="inlineStr">
         <is>
           <t>Option A</t>
         </is>
       </c>
-      <c r="G19" s="7" t="inlineStr"/>
-      <c r="H19" s="8" t="inlineStr">
+    </row>
+    <row r="37">
+      <c r="A37" s="6" t="inlineStr">
+        <is>
+          <t>Option C</t>
+        </is>
+      </c>
+      <c r="B37" s="8" t="inlineStr">
         <is>
           <t>Option A</t>
         </is>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="7" t="inlineStr"/>
-      <c r="B20" s="8" t="inlineStr">
-        <is>
-          <t>Option B</t>
-        </is>
-      </c>
-      <c r="D20" s="7" t="inlineStr"/>
-      <c r="E20" s="8" t="inlineStr">
-        <is>
-          <t>Option D</t>
-        </is>
-      </c>
-      <c r="G20" s="7" t="inlineStr"/>
-      <c r="H20" s="8" t="inlineStr">
-        <is>
-          <t>Option C</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="7" t="inlineStr"/>
-      <c r="B21" s="8" t="inlineStr">
-        <is>
-          <t>Option C</t>
-        </is>
-      </c>
-      <c r="D21" s="7" t="inlineStr"/>
-      <c r="E21" s="8" t="inlineStr">
-        <is>
-          <t>Option B</t>
-        </is>
-      </c>
-      <c r="G21" s="7" t="inlineStr"/>
-      <c r="H21" s="8" t="inlineStr">
-        <is>
-          <t>Option D</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="7" t="inlineStr"/>
-      <c r="B22" s="8" t="inlineStr">
-        <is>
-          <t>Option D</t>
-        </is>
-      </c>
-      <c r="D22" s="7" t="inlineStr"/>
-      <c r="E22" s="8" t="inlineStr">
-        <is>
-          <t>Option C</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="7" t="inlineStr"/>
-      <c r="B23" s="8" t="inlineStr">
-        <is>
-          <t>Option D</t>
-        </is>
-      </c>
-      <c r="D23" s="7" t="inlineStr"/>
-      <c r="E23" s="8" t="inlineStr">
-        <is>
-          <t>Option B</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="7" t="inlineStr"/>
-      <c r="B24" s="8" t="inlineStr">
+    <row r="38">
+      <c r="A38" s="6" t="inlineStr">
+        <is>
+          <t>Option C</t>
+        </is>
+      </c>
+      <c r="B38" s="8" t="inlineStr">
         <is>
           <t>Option A</t>
         </is>
       </c>
-      <c r="D24" s="7" t="inlineStr"/>
-      <c r="E24" s="8" t="inlineStr">
-        <is>
-          <t>Option C</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="7" t="inlineStr"/>
-      <c r="B25" s="8" t="inlineStr">
-        <is>
-          <t>Option A</t>
-        </is>
-      </c>
-      <c r="D25" s="7" t="inlineStr"/>
-      <c r="E25" s="8" t="inlineStr">
-        <is>
-          <t>Option D</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="7" t="inlineStr"/>
-      <c r="B26" s="8" t="inlineStr">
-        <is>
-          <t>Option C</t>
-        </is>
-      </c>
-      <c r="D26" s="7" t="inlineStr"/>
-      <c r="E26" s="8" t="inlineStr">
-        <is>
-          <t>Option D</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="7" t="inlineStr"/>
-      <c r="B27" s="8" t="inlineStr">
-        <is>
-          <t>Option A</t>
-        </is>
-      </c>
-      <c r="D27" s="7" t="inlineStr"/>
-      <c r="E27" s="8" t="inlineStr">
-        <is>
-          <t>Option A</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="7" t="inlineStr"/>
-      <c r="B28" s="8" t="inlineStr">
-        <is>
-          <t>Option D</t>
-        </is>
-      </c>
-      <c r="D28" s="7" t="inlineStr"/>
-      <c r="E28" s="8" t="inlineStr">
-        <is>
-          <t>Option A</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="7" t="inlineStr"/>
-      <c r="B29" s="8" t="inlineStr">
-        <is>
-          <t>Option D</t>
-        </is>
-      </c>
-      <c r="D29" s="7" t="inlineStr"/>
-      <c r="E29" s="8" t="inlineStr">
-        <is>
-          <t>Option C</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="7" t="inlineStr"/>
-      <c r="B30" s="8" t="inlineStr">
-        <is>
-          <t>Option B</t>
-        </is>
-      </c>
-      <c r="D30" s="7" t="inlineStr"/>
-      <c r="E30" s="8" t="inlineStr">
-        <is>
-          <t>Option A</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="7" t="inlineStr"/>
-      <c r="B31" s="8" t="inlineStr">
-        <is>
-          <t>Option D</t>
-        </is>
-      </c>
-      <c r="D31" s="7" t="inlineStr"/>
-      <c r="E31" s="8" t="inlineStr">
-        <is>
-          <t>Option D</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="7" t="inlineStr"/>
-      <c r="B32" s="8" t="inlineStr">
-        <is>
-          <t>Option C</t>
-        </is>
-      </c>
-      <c r="D32" s="7" t="inlineStr"/>
-      <c r="E32" s="8" t="inlineStr">
-        <is>
-          <t>Option D</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="7" t="inlineStr"/>
-      <c r="B33" s="8" t="inlineStr">
-        <is>
-          <t>Option D</t>
-        </is>
-      </c>
-      <c r="D33" s="7" t="inlineStr"/>
-      <c r="E33" s="8" t="inlineStr">
-        <is>
-          <t>Option B</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="7" t="inlineStr"/>
-      <c r="B34" s="8" t="inlineStr">
-        <is>
-          <t>Option B</t>
-        </is>
-      </c>
-      <c r="D34" s="7" t="inlineStr"/>
-      <c r="E34" s="8" t="inlineStr">
-        <is>
-          <t>Option D</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="7" t="inlineStr"/>
-      <c r="B35" s="8" t="inlineStr">
-        <is>
-          <t>Option D</t>
-        </is>
-      </c>
-      <c r="D35" s="7" t="inlineStr"/>
-      <c r="E35" s="8" t="inlineStr">
-        <is>
-          <t>Option C</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="7" t="inlineStr"/>
-      <c r="B36" s="8" t="inlineStr">
-        <is>
-          <t>Option A</t>
-        </is>
-      </c>
-      <c r="D36" s="7" t="inlineStr"/>
-      <c r="E36" s="8" t="inlineStr">
-        <is>
-          <t>Option D</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="7" t="inlineStr"/>
-      <c r="B37" s="8" t="inlineStr">
-        <is>
-          <t>Option A</t>
-        </is>
-      </c>
-      <c r="D37" s="7" t="inlineStr"/>
-      <c r="E37" s="8" t="inlineStr">
-        <is>
-          <t>Option B</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="7" t="inlineStr"/>
-      <c r="B38" s="8" t="inlineStr">
-        <is>
-          <t>Option A</t>
-        </is>
-      </c>
-      <c r="D38" s="7" t="inlineStr"/>
-      <c r="E38" s="8" t="inlineStr">
-        <is>
-          <t>Option D</t>
-        </is>
-      </c>
     </row>
     <row r="39">
-      <c r="A39" s="7" t="inlineStr"/>
+      <c r="A39" s="5" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
       <c r="B39" s="8" t="inlineStr">
         <is>
           <t>Option D</t>
         </is>
       </c>
-      <c r="D39" s="7" t="inlineStr"/>
-      <c r="E39" s="8" t="inlineStr">
-        <is>
-          <t>Option A</t>
-        </is>
-      </c>
     </row>
     <row r="40">
-      <c r="A40" s="7" t="inlineStr"/>
+      <c r="A40" s="6" t="inlineStr">
+        <is>
+          <t>Option C</t>
+        </is>
+      </c>
       <c r="B40" s="8" t="inlineStr">
         <is>
           <t>Option D</t>
-        </is>
-      </c>
-      <c r="D40" s="7" t="inlineStr"/>
-      <c r="E40" s="8" t="inlineStr">
-        <is>
-          <t>Option A</t>
         </is>
       </c>
     </row>
@@ -1095,7 +1027,7 @@
   <mergeCells count="1">
     <mergeCell ref="A5:E5"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update concise_ms csv pattern
</commit_message>
<xml_diff>
--- a/ans/result/1401CB01.xlsx
+++ b/ans/result/1401CB01.xlsx
@@ -642,10 +642,10 @@
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C11" s="6" t="n">
-        <v>-1</v>
+        <v>-1.2</v>
       </c>
       <c r="D11" s="7" t="n">
         <v>0</v>
@@ -659,15 +659,15 @@
         </is>
       </c>
       <c r="B12" s="5" t="n">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C12" s="6" t="n">
-        <v>-14</v>
+        <v>-16.8</v>
       </c>
       <c r="D12" s="7" t="n"/>
       <c r="E12" s="8" t="inlineStr">
         <is>
-          <t>42/112</t>
+          <t>53.2/140</t>
         </is>
       </c>
     </row>

</xml_diff>